<commit_message>
Updates from a few months
</commit_message>
<xml_diff>
--- a/rk_model/Data/Data_Yakou/Yakou_met_data_ITP_rk/input_data_env_variables.xlsx
+++ b/rk_model/Data/Data_Yakou/Yakou_met_data_ITP_rk/input_data_env_variables.xlsx
@@ -8048,7 +8048,7 @@
         <v>216.1805555555555</v>
       </c>
       <c r="H294">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="295" spans="1:8">
@@ -8074,7 +8074,7 @@
         <v>257.1201388888889</v>
       </c>
       <c r="H295">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="296" spans="1:8">
@@ -8100,7 +8100,7 @@
         <v>246.8354166666667</v>
       </c>
       <c r="H296">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="297" spans="1:8">
@@ -8126,7 +8126,7 @@
         <v>225.1083333333333</v>
       </c>
       <c r="H297">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="298" spans="1:8">
@@ -8152,7 +8152,7 @@
         <v>267.8986111111111</v>
       </c>
       <c r="H298">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="299" spans="1:8">
@@ -8178,7 +8178,7 @@
         <v>251.1756944444445</v>
       </c>
       <c r="H299">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="300" spans="1:8">
@@ -8204,7 +8204,7 @@
         <v>176.9541666666667</v>
       </c>
       <c r="H300">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="301" spans="1:8">
@@ -8230,7 +8230,7 @@
         <v>198.9597222222222</v>
       </c>
       <c r="H301">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="302" spans="1:8">
@@ -8256,7 +8256,7 @@
         <v>160.9041666666667</v>
       </c>
       <c r="H302">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="303" spans="1:8">
@@ -8282,7 +8282,7 @@
         <v>187.4069444444444</v>
       </c>
       <c r="H303">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="304" spans="1:8">
@@ -8308,7 +8308,7 @@
         <v>215.025</v>
       </c>
       <c r="H304">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="305" spans="1:8">
@@ -8334,7 +8334,7 @@
         <v>183.0069444444445</v>
       </c>
       <c r="H305">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="306" spans="1:8">
@@ -8360,7 +8360,7 @@
         <v>189.9708333333333</v>
       </c>
       <c r="H306">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="307" spans="1:8">
@@ -8386,7 +8386,7 @@
         <v>183.5465277777778</v>
       </c>
       <c r="H307">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="308" spans="1:8">
@@ -8412,7 +8412,7 @@
         <v>185.6631944444445</v>
       </c>
       <c r="H308">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="309" spans="1:8">
@@ -8438,7 +8438,7 @@
         <v>170.5826388888889</v>
       </c>
       <c r="H309">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -8464,7 +8464,7 @@
         <v>197.8638888888889</v>
       </c>
       <c r="H310">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="311" spans="1:8">
@@ -8490,7 +8490,7 @@
         <v>199.2722222222222</v>
       </c>
       <c r="H311">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="312" spans="1:8">
@@ -8516,7 +8516,7 @@
         <v>171.2486111111111</v>
       </c>
       <c r="H312">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="313" spans="1:8">
@@ -8542,7 +8542,7 @@
         <v>182.3138888888889</v>
       </c>
       <c r="H313">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="314" spans="1:8">
@@ -8568,7 +8568,7 @@
         <v>239.3472222222222</v>
       </c>
       <c r="H314">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="315" spans="1:8">
@@ -8594,7 +8594,7 @@
         <v>223.7847222222222</v>
       </c>
       <c r="H315">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="316" spans="1:8">
@@ -8620,7 +8620,7 @@
         <v>185.28125</v>
       </c>
       <c r="H316">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="317" spans="1:8">
@@ -8646,7 +8646,7 @@
         <v>160.0868055555555</v>
       </c>
       <c r="H317">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="318" spans="1:8">
@@ -8672,7 +8672,7 @@
         <v>144.1777777777778</v>
       </c>
       <c r="H318">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="319" spans="1:8">
@@ -8698,7 +8698,7 @@
         <v>149.5513888888889</v>
       </c>
       <c r="H319">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="320" spans="1:8">
@@ -8724,7 +8724,7 @@
         <v>188.1673611111111</v>
       </c>
       <c r="H320">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="321" spans="1:8">
@@ -8750,7 +8750,7 @@
         <v>202.4180555555556</v>
       </c>
       <c r="H321">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="322" spans="1:8">
@@ -8776,7 +8776,7 @@
         <v>205.5715277777778</v>
       </c>
       <c r="H322">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="323" spans="1:8">
@@ -8802,7 +8802,7 @@
         <v>206.5125</v>
       </c>
       <c r="H323">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="324" spans="1:8">
@@ -8828,7 +8828,7 @@
         <v>184.7159722222222</v>
       </c>
       <c r="H324">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="325" spans="1:8">
@@ -8854,7 +8854,7 @@
         <v>163.1736111111111</v>
       </c>
       <c r="H325">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="326" spans="1:8">
@@ -8880,7 +8880,7 @@
         <v>154.9638888888889</v>
       </c>
       <c r="H326">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -8906,7 +8906,7 @@
         <v>135.8423611111111</v>
       </c>
       <c r="H327">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="328" spans="1:8">
@@ -8932,7 +8932,7 @@
         <v>117.9125</v>
       </c>
       <c r="H328">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="329" spans="1:8">
@@ -8958,7 +8958,7 @@
         <v>131.18125</v>
       </c>
       <c r="H329">
-        <v>0</v>
+        <v>2.531569220430107E-07</v>
       </c>
     </row>
     <row r="330" spans="1:8">

</xml_diff>